<commit_message>
Add comprehensive testing framework with ICIJ validation and organized reporting
- Enhanced product_benchmark_tester.py with ICIJ validation using name_normalized field
- Added demo_oriented_tester.py for targeted testing with detailed criteria matching
- Updated excel_driven_regression_test.py with organized folder structure and UTF-8 encoding
- Added search_relevance_tester.py for search quality testing
- Added api_security_tester.py for API security testing
- Added security_test_queries.py with security test cases
- Enhanced consolidated_regression_test.py with improved reporting
- Added test data files and configuration
- Fixed character encoding issues in HTML reports
- Organized output folders with timestamp for better file management
- Cleaned up old report files
</commit_message>
<xml_diff>
--- a/GDC Old System Result.xlsx
+++ b/GDC Old System Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmallikarjuna/Documents/GDC automation test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E84710-A0C7-4E46-A6DA-06B48320EDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EF86DD-BA5F-3045-803E-0C96E81C72B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -146,13 +146,25 @@
   </si>
   <si>
     <t>AND CHARITIES; RIHS COMMITTEE FOR THE CALL AND GUIDANCE; RIHS-CAMBODIA; THE KUWAITI-CAMBODIAN ORPHANAGE CENTER; RIHS CAMBODIA-KUWAIT ORPHANAGE CENTER; RIHS CHAOM CHAU CENTER; THE KUWAIT-CAMBODIA ISLAMIC CULTURAL TRAINING CENTER; NARA WELFARE AND EDUCATION ASSOCIATION; RIHS-BOSNIA AND HERZEGOVINA; KUWAITI JOINT RELIEF COMMITTEE, BOSNIA AND HERZEGOVINA; KJRC-BOSNIA AND HERZEGOVINA; PLANDISTE SCHOOL, BOSNIA AND HERZEGOVINA; ORGANIZACIJA PREPORODA ISLAMSKE TRADICIJE KUVAJT; KUWAIT GENERAL COMMITTEE FOR AID; GENERAL KUWAIT COMMITTEE; RIHS-ALBANIA; CENTER OF CALL FOR WISDOM; CCFW; THIRRJA PER UTESI; NGO TURATH; RIHS-KOSOVO; DORA E MIRESISE; HAND OF MERCY; RIHS-AZERBAIJAN; RIHS-RUSSIA; RIHS-LEBANON; RIHS-BANGLADESH; RIHS-SOMALIA; RIHS-GHANA; RIHS-TANZANIA; RIHS-BENIN; RIHS-CAMEROON; RIHS-SENEGAL; RIHS-NIGERIA; RIHS-LIBERIA; RIHS-IVORY COAST; RIHS COMMITTEE FOR AFRICA","AltScript":"","RecType":"E"},{"recid":5929900,"ID":"20201350730","First_Name":"","Last_Name":"","Full_Name":"Societe Generale","Other_Names":"societegenerale.de.com; societe-generale.online","AltScript":"","RecType":"E"},{"recid":5943325,"ID":"20201381112","First_Name":"","Last_Name":"","Full_Name":"Generali Italia s.p.a.","Other_Names":"Societ\u00e0 Cattolica di Assicurazione s.p.a.","AltScript":"","RecType":"E"},{"recid":5943574,"ID":"20201381668","First_Name":"","Last_Name":"","Full_Name":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale","Other_Names":"","AltScript":"","RecType":"E"},{"recid":5950279,"ID":"20201390873","First_Name":"","Last_Name":"","Full_Name":"PAIN VICTOIRE","Other_Names":"PAINS VICTOIRE; SOCIETE GENERALE DE PAIN; SOCIETE GENERALE DES PAINS; PAN VICTOIRE; SOCIETE GENERAL DES PAINS SPRL","AltScript":"","RecType":"E"},{"recid":6083872,"ID":"20201470855","First_Name":"","Last_Name":"","Full_Name":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale Luxembourg","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6101509,"ID":"20201477707","First_Name":"","Last_Name":"","Full_Name":"CONTRATISTAS GENERALES &amp; INVERSIONES MERCURIO SOCIEDAD ANONIMA","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6134545,"ID":"20201493546","First_Name":"","Last_Name":"","Full_Name":"COMPRA VENTA &amp; SERVICIOS GENERALES SOCIEDAD ANONIMA CERRADA","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6145609,"ID":"20201498181","First_Name":"","Last_Name":"","Full_Name":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale SA","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6281038,"ID":"20201565615","First_Name":"","Last_Name":"","Full_Name":"Societe Generale","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6299209,"ID":"20201573090","First_Name":"","Last_Name":"","Full_Name":"CORDOVA CONTRATISTAS GENERALES SOCIEDAD ANONIMA CERRADA-C.O.R.S.A.C.","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6299272,"ID":"20201573146","First_Name":"","Last_Name":"","Full_Name":"GRUSAP CONTRATISTAS GENERALES SOCIEDAD ANONIMA CERRADA","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6393271,"ID":"20201613149","First_Name":"","Last_Name":"","Full_Name":"VISA COMPANY ASESORIA &amp; CONSULTORIA, CONTRATISTAS GENERALES SOCIEDAD ANONIMA CERRADA","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6450643,"ID":"20201636797","First_Name":"","Last_Name":"","Full_Name":"SERVICIOS GENERALES DHJC SOCIEDAD ANONIMA CERRADA","Other_Names":"SERVICIOS GENERALES DHJC S.A.C.","AltScript":"","RecType":"E"},{"recid":6532438,"ID":"20201665736","First_Name":"","Last_Name":"","Full_Name":"ESPINOZA CONTRATISTAS GENERALES SOCIEDAD ANONIMA","Other_Names":"CONSORCIO KALLPA: ESPINOZA CONTRATISTAS GENERALES SA","AltScript":"","RecType":"E"},{"recid":6562531,"ID":"20201677594","First_Name":"","Last_Name":"","Full_Name":"Societe Generale Securities Australia Pty Limited","Other_Names":"SGSAPL","AltScript":"","RecType":"E"},{"recid":6653875,"ID":"20201708217","First_Name":"","Last_Name":"","Full_Name":"CONTRATISTAS GENERALES IPARRAGUIRRE ALAYO SOCIEDAD ANONIMA CERRADA","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6654079,"ID":"20201708285","First_Name":"","Last_Name":"","Full_Name":"EDIFICACIONES MONTJOY O.CONTRATISTAS GENERALES SOCIEDAD ANONIMA - EDIMOCG S.A.","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6654901,"ID":"20201708559","First_Name":"","Last_Name":"","Full_Name":"MARINA &amp; HEREDIA GENERAL SERVICES SOCIEDAD ANONIMA CERRADA - M &amp; H GENERAL SERVICES S.A.C","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6655633,"ID":"20201708803","First_Name":"","Last_Name":"","Full_Name":"TRANSPORTES Y SERVICIOS GENERALES CUADROS-CESPEDES SOCIEDAD ANONIMA CERRADA","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6708418,"ID":"20201726501","First_Name":"","Last_Name":"","Full_Name":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale S.A.","Other_Names":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale","AltScript":"","RecType":"E"},{"recid":6773659,"ID":"20201161193","First_Name":"","Last_Name":"","Full_Name":"Societe Generale Financial Corporation","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6939613,"ID":"20201572833","First_Name":"","Last_Name":"","Full_Name":"JC CONSORCIO Y SERVICIOS GENERALES SOCIEDAD COMERCIAL DE RESPONSABILIDAD LIMITADA","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6945103,"ID":"20201781878","First_Name":"","Last_Name":"","Full_Name":"KIFAPA SERVICIOS GENERALES SOCIEDAD ANONIMA CERRADA","Other_Names":"KIFAPA SG S.A.C.","AltScript":"","RecType":"E"},{"recid":6946303,"ID":"20201782278","First_Name":"","Last_Name":"","Full_Name":"M &amp; A CONTRATISTAS GENERALES SOCIEDAD ANONIMA CERRADA","Other_Names":"M &amp; A CONTRATISTAS GENERALES S.A.C.","AltScript":"","RecType":"E"},{"recid":6946327,"ID":"20201782286","First_Name":"","Last_Name":"","Full_Name":"VAYMA ASESORES CONSULTORES GENERALES SOCIEDAD ANONIMA CERRADA","Other_Names":"VAYMA S.A.C.","AltScript":"","RecType":"E"},{"recid":6946462,"ID":"20201782331","First_Name":"","Last_Name":"","Full_Name":"CONTRATISTAS GENERALES IMAZA S.R.L.","Other_Names":"CONSTRUCTORA HNOS FEFER Y SERVICIOS GENERALES SOCIEDAD COMERCIAL DE RESPONSABILIDAD LIMITADA","AltScript":"","RecType":"E"},{"recid":6946909,"ID":"20201782480","First_Name":"","Last_Name":"","Full_Name":"AJL ESPINOZA SERVICIOS GENERALES SOCIEDAD ANONIMA CERRADA","Other_Names":"AJL ESPINOZA SERVICIOS GENERALES S.A.C.","AltScript":"","RecType":"E"},{"recid":6947131,"ID":"20201782554","First_Name":"","Last_Name":"","Full_Name":"MAFETSUR INVERSIONES GENERALES SOCIEDAD ANONIMA CERRADA","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6947173,"ID":"20201782568","First_Name":"","Last_Name":"","Full_Name":"RURAQ RAYLIN GENERAL SERVICES SOCIEDAD ANONIMA CERRADA","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6947221,"ID":"20201782584","First_Name":"","Last_Name":"","Full_Name":"ZEROBITS VENTAS Y SERVICIOS GENERALES SOCIEDAD COMERCIAL DE RESPONSABILIDAD LIMITADA","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6950110,"ID":"20201783547","First_Name":"","Last_Name":"","Full_Name":"JC CONSORCIO Y SERVICIOS GENERALES SOCIEDAD COMERCIAL DE RESPONSABILIDAD LIMITADA","Other_Names":"","AltScript":"","RecType":"E"},{"recid":7032868,"ID":"20201801728","First_Name":"","Last_Name":"","Full_Name":"Societe Generale Securities Australia Pty Ltd","Other_Names":"SGSAPL","AltScript":"","RecType":"E"}],"icij":[{"recid":14081,"ID":"80000014081","Full_Name":"SOCIETE GENERALE DES METAUX OCCIDENTAUX S.A.","otherNames":"","countries":"SWITZERLAND","activityType":"","relationships":""},{"recid":53044,"ID":"80000053044","Full_Name":"SOCIETE GENERALE DE GESTION ET SERVICES, S.A.","otherNames":"","countries":"JERSEY","activityType":"","relationships":""},{"recid":202442,"ID":"80000202442","Full_Name":"SOCIETE GENERALE D&amp;#039;INVESTISSEMENTS S.A.","otherNames":"","countries":"ISLE OF MAN","activityType":"","relationships":""},{"recid":259830,"ID":"80000259830","Full_Name":"Societe Generale Bank &amp;amp; Trust (Hong Kong office) -  ????????????","otherNames":"","countries":"","activityType":"Client Sundry Account","relationships":""},{"recid":272281,"ID":"80000272281","Full_Name":"Societe Generale Bank &amp;amp; Trust - (Singapore Office)","otherNames":"","countries":"","activityType":"Client Sundry Account","relationships":""},{"recid":322819,"ID":"80000322819","Full_Name":"SGS SOCIETE GENERALE DE SURVEILLANCE SA","otherNames":"","countries":"SWITZERLAND","activityType":"","relationships":"Intermediary of: ZURICH FINANCE GROUP LIMITED"},{"recid":323800,"ID":"80000323800","Full_Name":"SOCIETE GENERALE","otherNames":"","countries":"PANAMA","activityType":"","relationships":"Intermediary of: FIXTAIL CONSULTING INC.&lt;hr /&gt;Intermediary of: SPICELAB VENTURE INC.&lt;hr /&gt;Intermediary of: MAJOR CONSULTANS INC.&lt;hr /&gt;Intermediary of: GREENOCK INC.&lt;hr /&gt;Intermediary of: AMCAL MANAGING INC.&lt;hr /&gt;Intermediary of: SINFOVEST INC.&lt;hr /&gt;Intermediary of: FAIRFLY CONSULTANTS INC.&lt;hr /&gt;Intermediary of: MIDDLECROSS FINANCIAL CORPORATION INC.&lt;hr /&gt;Intermediary of: SCARA MANAGEMENT INC.&lt;hr /&gt;Intermediary of: CADIM MANAGEMENT INC.&lt;hr /&gt;Intermediary of: WALABI CONSULTANTS INC.&lt;hr /&gt;Intermediary of: CALANDO INTERNATIONAL INC.&lt;hr /&gt;Intermediary of: NILUX MANAGEMENT INC.&lt;hr /&gt;Intermediary of: EUROCASH MANAGERS INC.&lt;hr /&gt;Intermediary of: PATRISAFE INVESTMENTS INC.&lt;hr /&gt;Intermediary of: SPECTRUM MANAGEMENT INC.&lt;hr /&gt;Intermediary of: PANDORA MANAGEMENT INC.&lt;hr /&gt;Intermediary of: PABLANCA INVESTMENTS INC.&lt;hr /&gt;Intermediary of: CORPTRUST FINANCE INC.&lt;hr /&gt;Intermediary of: BULLOCK MANAGEMENT INC.&lt;hr /&gt;Intermediary of: FIRESTONE MANAGEMENT INC.&lt;hr /&gt;Intermediary of: ZODIAC CONSULTANTS INC.&lt;hr /&gt;Intermediary of: COROLLA INVESTMENTS INC.&lt;hr /&gt;Intermediary of: AGRIMINNA INC.&lt;hr /&gt;Intermediary of: WATERSIDE INTERNATIONAL INC.&lt;hr /&gt;Intermediary of: AQUACALDA INC.&lt;hr /&gt;Intermediary of: BLUEBERRY ASSOCIATES INC.&lt;hr /&gt;Intermediary of: TRANSIMATIC INC.&lt;hr /&gt;Intermediary of: PARSIFINE INC.&lt;hr /&gt;Intermediary of: VALEFIN INC.&lt;hr /&gt;Intermediary of: NADINVEST INC.&lt;hr /&gt;Intermediary of: PIPEFINE INC.&lt;hr /&gt;Intermediary of: ARROW CONSULTANTS INC.&lt;hr /&gt;Intermediary of: MATWICK MANAGERS INC.&lt;hr /&gt;Intermediary of: FLODIGAN INVESTMENTS INC.&lt;hr /&gt;Intermediary of: MARINE AND FISHING INTERNATIONAL AGENCY S.A.&lt;hr /&gt;Intermediary of: VALUDEC MANAGERS INC.&lt;hr /&gt;Intermediary of: SUDINTER HOLDINGS INC.&lt;hr /&gt;Intermediary of: HELLASSIN INC.&lt;hr /&gt;Intermediary of: BALLINVEST INTERNATIONAL INC.&lt;hr /&gt;Intermediary of: RACY HOLDING INC.&lt;hr /&gt;Intermediary of: STROMBOL CONSULTING INC.&lt;hr /&gt;Intermediary of: UNISTYLE CORPORATION INC.&lt;hr /&gt;Intermediary of: VALUEHOLD MANAGERS INC.&lt;hr /&gt;Intermediary of: PANTRANS CONSULTANTS INC&lt;hr /&gt;Intermediary of: TELECONTROL MANAGING INC.&lt;hr /&gt;Intermediary of: WHARRICK INTERNATIONAL INC.&lt;hr /&gt;Intermediary of: TERZA MANAGEMENT INC.&lt;hr /&gt;Intermediary of: CRYSTAL CONSULTANTS INTERNATIONAL INC.&lt;hr /&gt;Intermediary of: TIMOTHY INTERNATIONAL INC.&lt;hr /&gt;(And 46 more...)"},{"recid":324634,"ID":"80000324634","Full_Name":"SOCI\u00c9T\u00c9 G\u00c9N\u00c9RALE BANK &amp;amp; TRUST LUXEMBOURG","otherNames":"","countries":"LUXEMBOURG","activityType":"","relationships":"Intermediary of: MARELLE INC.&lt;hr /&gt;Intermediary of: UMEZA TRADING CORP.&lt;hr /&gt;Intermediary of: ALETTE INC.&lt;hr /&gt;Intermediary of: TALENT INC.&lt;hr /&gt;Intermediary of: SORRENTO CORP.&lt;hr /&gt;Intermediary of: ISART INVESTMENTS LTD.&lt;hr /&gt;Intermediary of: KNICKLE INTERNATIONAL LIMITED&lt;hr /&gt;Intermediary of: ASPENDALE HOLDINGS INC.&lt;hr /&gt;Intermediary of: ILFORT VENTURES S.A.&lt;hr /&gt;Intermediary of: RAMBURY CORP.&lt;hr /&gt;Intermediary of: ANTES PROMOTION LTD.&lt;hr /&gt;Intermediary of: JULUCA HOLDINGS LIMITED&lt;hr /&gt;Intermediary of: GAVROCHE EQUITIES S.A.&lt;hr /&gt;Intermediary of: AIMEE INVESTMENT CORP.&lt;hr /&gt;Intermediary of: TRENVILLE S.A.&lt;hr /&gt;Intermediary of: FUNKYTOWN LIMITED&lt;hr /&gt;Intermediary of: VALENTINO TECHNOLOGIES INC.&lt;hr /&gt;Intermediary of: OCANTA INC.&lt;hr /&gt;Intermediary of: CURONA INC.&lt;hr /&gt;Intermediary of: IRTIS INC.&lt;hr /&gt;Intermediary of: FORPORT INC.&lt;hr /&gt;Intermediary of: LAZIO REAL ESTATE INC.&lt;hr /&gt;Intermediary of: UNIVERSAL EXPORTS S.A.&lt;hr /&gt;Intermediary of: VALOR INVESTORS INC.&lt;hr /&gt;Intermediary of: VALISE LTD.&lt;hr /&gt;Intermediary of: SOLERO INC.&lt;hr /&gt;Intermediary of: CHANTILLY GROUP S.A.&lt;hr /&gt;Intermediary of: HORTENSIA INC.&lt;hr /&gt;Intermediary of: PANTRANS CONSULTANTS INC.&lt;hr /&gt;Intermediary of: CARNEOL S.A.&lt;hr /&gt;Intermediary of: CHAMPS INC.&lt;hr /&gt;Intermediary of: CRISTAL INC.&lt;hr /&gt;Intermediary of: LIMONE CORP.&lt;hr /&gt;Intermediary of: NADIS TRADING CORP.&lt;hr /&gt;Intermediary of: CAJOU GLOBAL S.A.&lt;hr /&gt;Intermediary of: MIXIT INC.&lt;hr /&gt;Intermediary of: ILIAD HOLDINGS LIMITED&lt;hr /&gt;Intermediary of: COMMONLANDS LLC&lt;hr /&gt;Intermediary of: INGO TREE S.A.&lt;hr /&gt;Intermediary of: AQUARIS INC.&lt;hr /&gt;Intermediary of: ATTEC S.A.&lt;hr /&gt;Intermediary of: OXLEYS MANAGEMENT INC.&lt;hr /&gt;Intermediary of: RISKWORLD INVESTMENTS INC.&lt;hr /&gt;Intermediary of: CALELLA LIMITED&lt;hr /&gt;Intermediary of: DORSAN INC.&lt;hr /&gt;Intermediary of: BAMERA CORP.&lt;hr /&gt;Intermediary of: DIXI CORP.&lt;hr /&gt;Intermediary of: HILRIL S.A.&lt;hr /&gt;Intermediary of: CAPUA CORP.&lt;hr /&gt;Intermediary of: VALCO ASSETS LTD.&lt;hr /&gt;(And 415 more...)"},{"recid":324851,"ID":"80000324851","Full_Name":"SOCI\u00c9T\u00c9 G\u00c9N\u00c9RALE BANK &amp;amp; TRUST LUXEMBOURG","otherNames":"","countries":"","activityType":"","relationships":"Intermediary of: VALVERT FOUNDATION&lt;hr /&gt;Intermediary of: ROUSSEAU FOUNDATION"},{"recid":325875,"ID":"80000325875","Full_Name":"SOCIETE GENERALE","otherNames":"","countries":"UNITED KINGDOM","activityType":"","relationships":"Intermediary of: AMITEC IMPORT/EXPORT S.A.&lt;hr /&gt;Intermediary of: COLORAMA ENTERPRISES S.A."},{"recid":329245,"ID":"80000329245","Full_Name":"SOCIETE GENERALE D&amp;#039;INVESTISSEMENTS S.A..","otherNames":"","countries":"MONACO","activityType":"","relationships":"Intermediary of: CORIANA HOLDING S. A."},{"recid":340256,"ID":"80000340256","Full_Name":"Societe Generale Bank &amp;amp; Trust (Hong Kong office) -  ????????????","otherNames":"","countries":"HONG KONG","activityType":"","relationships":"Intermediary of: CLEAR TECH GROUP LIMITED&lt;hr /&gt;Intermediary of: SUCCESS MEDIA LIMITED&lt;hr /&gt;Intermediary of: NEXT MEDIA TECHNOLOGY LIMITED&lt;hr /&gt;Intermediary of: Spirit Capital Group Limited&lt;hr /&gt;Intermediary of: SOUTH WINDMILL LIMITED&lt;hr /&gt;Intermediary of: TOTAL TALENT GROUP LIMITED&lt;hr /&gt;Intermediary of: ELITE LAND TECHNOLOGY LIMITED&lt;hr /&gt;Intermediary of: PRINCE PATH GROUP LIMITED&lt;hr /&gt;Intermediary of: MAGIC KING DEVELOPMENT LIMITED&lt;hr /&gt;Intermediary of: KING PROFIT SERVICES LIMITED&lt;hr /&gt;Intermediary of: Delightful Cheers Limited&lt;hr /&gt;Intermediary of: SUPER STRATEGY LIMITED&lt;hr /&gt;Intermediary of: Grandview Technology Limited&lt;hr /&gt;Intermediary of: VastChina International Capital Group Limited&lt;hr /&gt;Intermediary of: POLY SUCCESS ENTERPRISES LIMITED&lt;hr /&gt;Intermediary of: Societe Generale Bank &amp;amp; Trust (Hong Kong office) -  ????????????&lt;hr /&gt;Intermediary of: STS Management Ltd.&lt;hr /&gt;Intermediary of: COASTLINE ENTERPRISES GROUP LIMITED&lt;hr /&gt;Intermediary of: DRAGON MILLION GROUP LIMITED&lt;hr /&gt;Intermediary of: Skyview Technology Limited&lt;hr /&gt;Intermediary of: Gala Holding Investment Limited&lt;hr /&gt;Intermediary of: LOTUS BUSHES LIMITED&lt;hr /&gt;Intermediary of: CRYSTAL POINT DEVELOPMENT LIMITED&lt;hr /&gt;Intermediary of: BRILLIANCE SOUND LIMITED&lt;hr /&gt;Intermediary of: SKAGEN INTERNATIONAL LIMITED&lt;hr /&gt;Intermediary of: Micro Development Ltd.&lt;hr /&gt;Intermediary of: Agape International Limited&lt;hr /&gt;Intermediary of: SUNVIEW SPARKLE ASSET MANAGEMENT LIMITED&lt;hr /&gt;Intermediary of: ELITE CITY TRADING LIMITED&lt;hr /&gt;Intermediary of: BEST GRADE TECHNOLOGY LIMITED&lt;hr /&gt;Intermediary of: HUGH FORCE TECHNOLOGY LIMITED&lt;hr /&gt;Intermediary of: Sunshine Investment Corp.&lt;hr /&gt;Intermediary of: Mega Tec Inc.&lt;hr /&gt;Intermediary of: THOUSAND PERFUME TRADING LIMITED&lt;hr /&gt;Intermediary of: Guardtek Group Corp&lt;hr /&gt;Intermediary of: Ironwill Industrial Corp&lt;hr /&gt;Intermediary of: TK&amp;amp;J International Corp.&lt;hr /&gt;Intermediary of: JK&amp;amp;J International Corp.&lt;hr /&gt;Intermediary of: PK&amp;amp;J International Corp.&lt;hr /&gt;Intermediary of: RIGHT ELEMENTS TECHNOLOGY LIMITED&lt;hr /&gt;Intermediary of: PACIFIC CAPITAL RESOURCES, LTD.&lt;hr /&gt;Intermediary of: CLEVER IDEAS INTERNATIONAL LIMITED"},{"recid":340423,"ID":"80000340423","Full_Name":"Societe Generale Bank &amp;amp; Trust - (Singapore Office)","otherNames":"","countries":"SINGAPORE","activityType":"","relationships":"Intermediary of: Brave Stone International Development Ltd&lt;hr /&gt;Intermediary of: Cross Country Ventures Ltd&lt;hr /&gt;Intermediary of: United Energy Trading Limited&lt;hr /&gt;Intermediary of: Contract Design &amp;amp; Systems Furniture Specialist Inc.&lt;hr /&gt;Intermediary of: Healthkeepers Ventures Inc.&lt;hr /&gt;Intermediary of: Sedai Corp&lt;hr /&gt;Intermediary of: CONVENTRY HOLDING COMPANY LTD&lt;hr /&gt;Intermediary of: FAMILY ASSET INVESTMENT COMPANY LTD&lt;hr /&gt;Intermediary of: Everbloom Asset Management Inc.&lt;hr /&gt;Intermediary of: Cogent Capital Corporation&lt;hr /&gt;Intermediary of: THESTRAL LIMITED&lt;hr /&gt;Intermediary of: ORO Corporation&lt;hr /&gt;Intermediary of: Digital Era Trading Inc.&lt;hr /&gt;Intermediary of: Focal View Group Limited&lt;hr /&gt;Intermediary of: Societe Generale Bank &amp;amp; Trust - (Singapore Office)&lt;hr /&gt;Intermediary of: Alpha Centauri Development Inc.&lt;hr /&gt;Intermediary of: Elgin Wealth Management Inc.&lt;hr /&gt;Intermediary of: SPRINGWELL VENTURES LTD&lt;hr /&gt;Intermediary of: Capitol Equities Ltd&lt;hr /&gt;Intermediary of: DIRGANTARA INDONESIA (Indonesian Aerospace, IAe-BSID) LTD&lt;hr /&gt;Intermediary of: Maple Gold Trading Ltd&lt;hr /&gt;Intermediary of: Summit Holdings Group Worldwide Limited&lt;hr /&gt;Intermediary of: Jian Tai Engineering Consultants Ltd&lt;hr /&gt;Intermediary of: Timeless Assets Overseas Ltd&lt;hr /&gt;Intermediary of: GLOBAL CREST (ASIA) PTE LTD&lt;hr /&gt;Intermediary of: Beaupoint International Inc.&lt;hr /&gt;Intermediary of: Starshine Assets Ltd&lt;hr /&gt;Intermediary of: Portal Growth Ltd&lt;hr /&gt;Intermediary of: E-vent Ltd&lt;hr /&gt;Intermediary of: Star Performance International Ltd&lt;hr /&gt;Intermediary of: Ad-Assets Ltd&lt;hr /&gt;Intermediary of: JAMES AND MITCHELL PARTNERS LIMITED&lt;hr /&gt;Intermediary of: THOMAS BARNEY ADVISORS LIMITED&lt;hr /&gt;Intermediary of: Prairie Development Ltd&lt;hr /&gt;Intermediary of: Global Wealth Capital Ltd&lt;hr /&gt;Intermediary of: PTC Investment Ltd.&lt;hr /&gt;Intermediary of: Kings Gate International Ltd&lt;hr /&gt;Intermediary of: Truck Body Parts Industrial Co. Ltd&lt;hr /&gt;Intermediary of: Universal Wealth Group Ltd&lt;hr /&gt;Intermediary of: Specific Assets Ltd&lt;hr /&gt;Intermediary of: Liquid Products Ltd&lt;hr /&gt;Intermediary of: Lian An Corporation&lt;hr /&gt;Intermediary of: ACME INTERNATIONAL GROUP LTD&lt;hr /&gt;Intermediary of: GLORY DRAGON INVESTMENTS GROUP LIMITED&lt;hr /&gt;Intermediary of: Trinity Investment Ventures Limited&lt;hr /&gt;Intermediary of: Investsmart International Inc.&lt;hr /&gt;Intermediary of: PPF TRADE CO., LTD.&lt;hr /&gt;Intermediary of: Hermitage Capital Planners Ltd"},{"recid":416119,"ID":"80000416119","Full_Name":"Societe Generale Bank &amp;amp; Trust","otherNames":"","countries":"LUXEMBOURG","activityType":"","relationships":"Shareholder of: BRIDGEWATER INTERNATIONAL HOLDINGS INC.&lt;hr /&gt;Similar name and address as: Societe Generale Bank &amp;amp; Trust"},{"recid":431068,"ID":"80000431068","Full_Name":"Societe Generale Bank &amp;amp; Trust","otherNames":"","countries":"LUXEMBOURG","activityType":"","relationships":"Shareholder of: COPAFI HOLDING S.A.&lt;hr /&gt;Shareholder of: FINALUX HOLDING S.A."},{"recid":435217,"ID":"80000435217","Full_Name":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale Bank &amp;amp; Trust","otherNames":"","countries":"LUXEMBOURG","activityType":"","relationships":"Shareholder of: FOSTAR INVEST LTD.&lt;hr /&gt;Shareholder of: SOFTWARE MAINTENANCE CORP."},{"recid":435218,"ID":"80000435218","Full_Name":"Societe Generale Bank &amp;amp; Trust","otherNames":"","countries":"LUXEMBOURG","activityType":"","relationships":"Shareholder of: BRIDGEWATER INTERNATIONAL HOLDINGS INC."},{"recid":438238,"ID":"80000438238","Full_Name":"BEARER Holder as depositary: Soci\u00e9t\u00e9 G\u00e9n\u00e9rale Bank &amp;amp; Trust","otherNames":"","countries":"LUXEMBOURG","activityType":"","relationships":"Shareholder of: SANTORIN LIMITED"},{"recid":439278,"ID":"80000439278","Full_Name":"BEARER Holder as depositary : Soci\u00e9t\u00e9 G\u00e9n\u00e9rale Bank &amp;amp; Trust","otherNames":"","countries":"LUXEMBOURG","activityType":"","relationships":"Shareholder of: SANTORIN LIMITED&lt;hr /&gt;Similar name and address as: BEARER Holder as depositary: Soci\u00e9t\u00e9 G\u00e9n\u00e9rale Bank &amp;amp; Trust"},{"recid":535830,"ID":"80000535830","Full_Name":"SGS Soci\u00e9t\u00e9 G\u00e9n\u00e9rale de Surveillance SA","otherNames":"","countries":"SWITZERLAND","activityType":"","relationships":"Shareholder of: ZURICH FINANCE GROUP LIMITED"},{"recid":553758,"ID":"80000553758","Full_Name":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale Private Banking (Suisse) SA","otherNames":"","countries":"SWITZERLAND","activityType":"","relationships":"Shareholder of: AMBRETTE INC."},{"recid":686018,"ID":"80000686018","Full_Name":"Societe Generale Asia Limited","otherNames":"","countries":"HONG KONG","activityType":"","relationships":"Shareholder of: Global Development Services Ltd.&lt;hr /&gt;Shareholder of: Phoenix Development Services Limited&lt;hr /&gt;Shareholder of: Basic Development Services Limited"}],"mex":[{"recid":3633013,"ID":"30590147323","First_Name":"","Last_Name":"","Full_Name":"SOCIEDAD COOPERATIVA DE PRODUCCION PESQUERA GENERAL ANSELMO MACIAS VALENZUELA SCL","Other_Names":"","AltScript":"","RecType":"E"},{"recid":3737224,"ID":"30580020259","First_Name":"","Last_Name":"","Full_Name":"SOCIEDAD INTEGRADORA DEL TRANSPORTE PUBLICO GENERAL FRANCISCO VILLA S.A DE C.V.","Other_Names":"","AltScript":"","RecType":"E"},{"recid":3829465,"ID":"30580074730","First_Name":"","Last_Name":"","Full_Name":"SOCIEDAD COOPERATIVA DE PRODUCCION PESQUERA GENERAL ANSELMO MACIAS VALENZUELA SCL","Other_Names":"","AltScript":"","RecType":"E"}],"soe":[{"recid":394345,"ID":"90100000792","Full_Name":"PARCO GENETICO DELL'OGLIASTRA SOCIETA' CONSORTILE A RESPONSABILITA' LIMITATA","Other_Names":"PARCO GEN.O.S. CONS. A R.L.","AltScript":"","Owner_Name":"Perdasdefogu (OG)","Address_Country":"Italy","RecType":"E"},{"recid":418021,"ID":"90100001289","Full_Name":"SO.GE.A. SOCIETA' GENERALE ECOLOGIA AMBIENTE SRL","Other_Names":"","AltScript":"","Owner_Name":"Calvatone (CR)","Address_Country":"Italy","RecType":"E"},{"recid":430150,"ID":"90100004678","Full_Name":"GENE.S.I.SOCIETA' GENERALE PER LA GESTIONE DEI SERVIZI ALLE IMPRESE S.C.R.L.","Other_Names":"","AltScript":"","Owner_Name":"Torre Annunziata (NA)","Address_Country":"Italy","RecType":"E"},{"recid":431038,"ID":"90100004410","Full_Name":"SOCIETA' GENERALE TRASPORTI E MOBILITA' - S.P.A.","Other_Names":"SGTM - S.P.A.","AltScript":"","Owner_Name":"Pistoia (PT)","Address_Country":"Italy","RecType":"E"},{"recid":432802,"ID":"90100005492","Full_Name":"AZIENDA ENERGETICA FALZES SOCIETA' COOPERATIVA","Other_Names":"ENERGIEWERK PFALZEN GENOSSENSCHAFT IN KURZFORM EWP GEN.","AltScript":"","Owner_Name":"Falzes (BZ)","Address_Country":"Italy","RecType":"E"},{"recid":475237,"ID":"90100060002","Full_Name":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale Congo","Other_Names":"SG-Congo","AltScript":"","Owner_Name":"Government of Republic of the Congo","Address_Country":"Republic of the Congo","RecType":"E"},{"recid":540316,"ID":"90100000067","Full_Name":"ASSICURAZIONI GENERALI - SOCIETA' PER AZIONI","Other_Names":"","AltScript":"","Owner_Name":"Trieste (TS)","Address_Country":"Italy","RecType":"E"},{"recid":613795,"ID":"90100125586","Full_Name":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale Tchad","Other_Names":"SGT","AltScript":"","Owner_Name":"Government of Chad","Address_Country":"Chad","RecType":"E"},{"recid":636145,"ID":"90100007297","Full_Name":"Trenes Argentinos Capital Humano","Other_Names":"Desarrollo del Capital Humano Ferroviario Sociedad An\u00f3nima de Participaci\u00f3n Estatal Mayoritaria; Desarrollo del Capital Humano Ferroviario S.A.; DECAHF; Argentine Trains Human Capital; Administradora de Recursos Humanos Ferroviarios Sociedad An\u00f3nima con Participaci\u00f3n Estatal Mayoritaria; Administradora de Recursos Humanos Ferroviarios S.A.; Trenes Argentinos Recursos Humanos; Ferrocarril General Belgrano Sociedad An\u00f3nima; FGBSA; Argentine Trains Human Resources","AltScript":"","Owner_Name":"Ministry of Transport","Address_Country":"Argentina","RecType":"E"},{"recid":636271,"ID":"90100007310","Full_Name":"Administraci\u00f3n General de Puertos Sociedad del Estado","Other_Names":"Administraci\u00f3n General de Puertos S.E.; Administraci\u00f3n General de Puertos; Puerto Buenos Aires; AGP; AGPSE","AltScript":"","Owner_Name":"Ministry of Transport","Address_Country":"Argentina","RecType":"E"},{"recid":636850,"ID":"90100007307","Full_Name":"Fabricaciones Militares Sociedad del Estado","Other_Names":"Direcci\u00f3n General de Fabricaciones Militares; DGFM; Fabricaciones Militares","AltScript":"","Owner_Name":"Ministry of Defense","Address_Country":"Argentina","RecType":"E"},{"recid":718180,"ID":"90100055568","Full_Name":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale Maritime","Other_Names":"GEMA; Societe Generale Maritime","AltScript":"\u0634\u0631\u0643\u0629 \u062c\u0646\u0631\u0627\u0644 \u0627\u0644\u0628\u062d\u0631\u064a\u0629; \u062c\u064a\u0645\u0627","Owner_Name":"Groupe Alg\u00e9rien de Transport Maritime","Address_Country":"Algeria","RecType":"E"},{"recid":719881,"ID":"90100034662","Full_Name":"Sociedad General de las Bah\u00edas de C\u00e1diz y Algeciras, S.A.","Other_Names":"Sociedad General de las Bah\u00edas de C\u00e1diz y Algeciras SA","AltScript":"","Owner_Name":"Spain","Address_Country":"Spain","RecType":"E"},{"recid":835108,"ID":"90100106491","Full_Name":"National Health Insurance of Nantan General Hospital Societies","Other_Names":"","AltScript":"\u56fd\u6c11\u5065\u5eb7\u4fdd\u967a\u5357\u4e39\u75c5\u9662\u7d44\u5408; \u30b3\u30af\u30df\u30f3\u30b1\u30f3\u30b3\u30a6\u30db\u30b1\u30f3\u30ca\u30f3\u30bf\u30f3\u30d3\u30e7\u30a6\u30a4\u30f3\u30af\u30df\u30a2\u30a4","Owner_Name":"Kyoto","Address_Country":"Japan","RecType":"E"},{"recid":838036,"ID":"90100020636","Full_Name":"Soci\u00e9t\u00e9 Generale Thermique","Other_Names":"","AltScript":"","Owner_Name":"France","Address_Country":"France","RecType":"E"},{"recid":861175,"ID":"90100001471","Full_Name":"SOCIETA' GENERALE PER LA GESTIONE DEL POLO TECNOLOGICO CONCIARIO SOCIETA' CONSORTILE A RESPONSABILITA' LIMITATA","Other_Names":"PO.TE.CO. S.C.R.L.","AltScript":"","Owner_Name":"Castelfranco Di Sotto (PI)","Address_Country":"Italy","RecType":"E"},{"recid":864910,"ID":"90100004415","Full_Name":"SOCIETA' ITALIANA COSTRUZIONI GENERALI S.R.L. - S.I.CO.GEN. (O SEMPLICEMENTE*S.I.CO.GEN. S.R.L.)","Other_Names":"","AltScript":"","Owner_Name":"Torino","Address_Country":"Italy","RecType":"E"},{"recid":868639,"ID":"90100068198","Full_Name":"Societ\u00e0 Generale d'Informatica S.p.A.","Other_Names":"Societ\u00e0 Generale d'Informatica S.p.A.; Sogei S.p.A.","AltScript":"","Owner_Name":"Ministry of Economy and Finance","Address_Country":"Italy","RecType":"E"},{"recid":943999,"ID":"90100040719","Full_Name":"National Societe Generale Bank Egypt","Other_Names":"National Soci\u00e9t\u00e9 G\u00e9n\u00e9rale Bank; NSGB","AltScript":"\u0627\u0644\u0628\u0646\u0643 \u0627\u0644\u0623\u0647\u0644\u064a \u0633\u0648\u0633\u064a\u062a\u064a\u0647 \u062c\u0646\u0631\u0627\u0644","Owner_Name":"Qatar National Bank","Address_Country":"Egypt","RecType":"E"},{"recid":945109,"ID":"90100049689","Full_Name":"Soci\u00e9t\u00e9 Anonyme Mon\u00e9gasque G\u00e9n\u00e9rale d'H\u00f4tellerie","Other_Names":"Monegasque General Anonymous Society of Hotels; SOGETEL","AltScript":"","Owner_Name":"Soci\u00e9t\u00e9 Anonyme des Bains de Mer et du Cercle des \u00c9trangers \u00e0 Monaco","Address_Country":"Monaco","RecType":"E"},{"recid":950194,"ID":"90100020131","Full_Name":"Orano Projets","Other_Names":"Soci\u00e9t\u00e9 g\u00e9n\u00e9rale pour les techniques nouvelles; SGN","AltScript":"","Owner_Name":"Orano S.A.","Address_Country":"France","RecType":"E"},{"recid":965620,"ID":"90100089644","Full_Name":"Soci\u00e9t\u00e9 La G\u00e9n\u00e9rale des Ventes","Other_Names":"STE LA GENERALE DE VENTE; G\u00c9N\u00c9RALE DE VENTE; \u00abGEVE\u00bb; La g\u00e9n\u00e9rale des ventes","AltScript":"\u0627\u0644\u0634\u0631\u0643\u0629 \u0627\u0644\u0639\u0627\u0645\u0629 \u0644\u0644\u0628\u064a\u0639","Owner_Name":"Banque Nationale Agricole","Address_Country":"Tunisia","RecType":"E"},{"recid":978805,"ID":"90100022046","Full_Name":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale d'Entreprise de Mat\u00e9riel et de Travaux","Other_Names":"SOMATRA-GET; SOMATRAGET; General Entreprise of Material and Works Company; Soci\u00e9t\u00e9 G\u00e9n\u00e9rale d'Entreprises, de Mat\u00e9riels et de Travaux (SOMATRA-GET)","AltScript":"\u0627\u0644\u0634\u0631\u0643\u0629 \u0627\u0644\u0639\u0627\u0645\u0629 \u0644\u0644\u0645\u0642\u0627\u0648\u0644\u0627\u062a \u0648\u0627\u0644\u0645\u0639\u062f\u0627\u062a \u0648\u0627\u0644\u0623\u0634\u063a\u0627\u0644 \u0633\u0648\u0645\u0627\u062a\u0631\u0627- \u062c\u0627\u062a","Owner_Name":"Government of Tunisia","Address_Country":"Tunisia","RecType":"E"},{"recid":991309,"ID":"90100089661","Full_Name":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale d'Etudes de Supervision et de Travaux","Other_Names":"SOGEST; SOGEST SA","AltScript":"\u0627\u0644\u062c\u0645\u0639\u064a\u0629 \u0627\u0644\u0639\u0627\u0645\u0629 \u0644\u0644\u062f\u0631\u0627\u0633\u0627\u062a \u0648 \u0627\u0644\u0645\u0631\u0627\u0642\u0628\u0629 \u0648 \u0627\u0644\u0639\u0645\u0644","Owner_Name":"Banque Nationale Agricole","Address_Country":"Tunisia","RecType":"E"}],"rights":[{"recid":178819,"ID":"30710016919","First_Name":"","Last_Name":"","Full_Name":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale","Other_Names":"","AltScript":"","RecType":"E"},{"recid":178822,"ID":"30710016920","First_Name":"","Last_Name":"","Full_Name":"Soci\u00e9t\u00e9 G\u00e9n\u00e9rale de Surveillance","Other_Names":"SGS","AltScript":"","RecType":"E"},{"recid":178825,"ID":"30710016921","First_Name":"","Last_Name":"","Full_Name":"Societe Generale Equipment Finance Limited","Other_Names":"","AltScript":"","RecType":"E"}],"col":[],"media":[],"ofac":[]}}}],"Redirect":null}</t>
+  </si>
+  <si>
+    <t>Mirage Air craft Services</t>
+  </si>
+  <si>
+    <t>{"Result":1,"ErrTitle":"","ErrMsg":"","ErrMsgWidth":null,"ErrBtnLabel":"Ok","MultiErr":null,"AppNotice":null,"FuncName":null,"Args":[{"nameSearch":{"SearchResult":{"timestamp":"2025-09-17 14:30:18","firstName":"","lastName":"","fullName":"Mirage Air craft Services","type":"E","method":3,"tokens":{"first":[],"first_syn":[],"last":[],"last_syn":[],"full":["MIRAGE","AIR","CRAFT","SERVICES"],"full_syn":{"MIRAGE":[],"AIR":["AEREA","AEREO","AEREOS","EIR"],"CRAFT":[],"SERVICES":["SERV","SERVICIO","SERVICIOS","SERVICOS","SERVICE"]},"icij_name":["MIRAGE","AIR","CRAFT","SERVICES"],"icij_nameSyn":{"MIRAGE":[],"AIR":["AEREA","AEREO","AEREOS","EIR"],"CRAFT":[],"SERVICES":["SERV","SERVICIO","SERVICIOS","SERVICOS","SERVICE"]}},"deflated":"MIRAGEAIRCRAFTSERVICES","generated":{"pep":"2025-07-22 16:47:11","sanction":"2025-09-09 15:05:21","watch":"2025-08-07 17:33:59","mex":"2025-07-31 13:34:08","soe":"2025-06-18 10:36:28","rights":"2025-07-31 13:47:27","col":"2025-07-31 13:42:51","icij":"2016-07-15 00:00:00"},"matches":2,"hits":3,"ref":{"sanction":["361804:10131047950"],"watch":["6306178:20201576120","6444316:20201633423"]},"runtime":{"pep":0.007000000000000000145716771982051795930601656436920166015625,"sanction":0.00899999999999999931998839741709161899052560329437255859375,"watch":0.008000000000000000166533453693773481063544750213623046875,"mex":0.00899999999999999931998839741709161899052560329437255859375,"soe":0.007000000000000000145716771982051795930601656436920166015625,"rights":0.0120000000000000002498001805406602215953171253204345703125,"col":0.00899999999999999931998839741709161899052560329437255859375,"icij":0.00600000000000000012490009027033011079765856266021728515625},"error":"","countryExcl":"","listExcl":"","sqlTemplate":"SELECT DISTINCT L1.recid\nFROM {_tbl_} AS L1{filter_join}\nINNER JOIN {_tbl_} AS L2 ON L2.recid = L1.recid\nINNER JOIN {_tbl_} AS L3 ON L3.recid = L1.recid\nINNER JOIN {_tbl_} AS L4 ON L4.recid = L1.recid\nWHERE {filter_cond}L1.token = 'MIRAGE'\nAND (L2.token = 'AIR'\n  OR L2.token = 'AEREA'\n  OR L2.token = 'AEREO'\n  OR L2.token = 'AEREOS'\n  OR L2.token = 'EIR'\n)\nAND L3.token = 'CRAFT'\nAND (L4.token = 'SERVICES'\n  OR L4.token = 'SERV'\n  OR L4.token = 'SERVICIO'\n  OR L4.token = 'SERVICIOS'\n  OR L4.token = 'SERVICOS'\n  OR L4.token = 'SERVICE'\n)\nLIMIT 100","deflatedSqlTemplate":"SELECT DISTINCT L1.recid\nFROM {_tbl_} AS L1{filter_join}\nWHERE {filter_cond}L1.token = 'MIRAGEAIRCRAFTSERVICES'\nAND L1.nameSrc = 'Deflated'\n LIMIT 100","nameID":3341266,"icijName":"Mirage Air craft Services","sqlTemplate_icij":"SELECT DISTINCT L1.recid\nFROM {_tbl_} AS L1\nINNER JOIN {_tbl_} AS L2 ON L2.recid = L1.recid\nINNER JOIN {_tbl_} AS L3 ON L3.recid = L1.recid\nINNER JOIN {_tbl_} AS L4 ON L4.recid = L1.recid\nLEFT JOIN {_tbl_} AS deflateJoin ON deflateJoin.recid = L1.recid\nWHERE L1.token = 'MIRAGE'\nAND (L2.token = 'AIR'\n  OR L2.token = 'AEREA'\n  OR L2.token = 'AEREO'\n  OR L2.token = 'AEREOS'\n  OR L2.token = 'EIR'\n)\nAND L3.token = 'CRAFT'\nAND (L4.token = 'SERVICES'\n  OR L4.token = 'SERV'\n  OR L4.token = 'SERVICIO'\n  OR L4.token = 'SERVICIOS'\n  OR L4.token = 'SERVICOS'\n  OR L4.token = 'SERVICE'\n)\nAND deflateJoin.token LIKE '%MIRAGEAIRCRAFTSERVICES%'\nLIMIT 100"},"code":"Array\n(\n    [timestamp] =&gt; 2025-09-17 14:30:18\n    [firstName] =&gt; \n    [lastName] =&gt; \n    [fullName] =&gt; Mirage Air craft Services\n    [type] =&gt; E\n    [method] =&gt; 3\n    [tokens] =&gt; Array\n        (\n            [first] =&gt; Array\n                (\n                )\n\n            [first_syn] =&gt; Array\n                (\n                )\n\n            [last] =&gt; Array\n                (\n                )\n\n            [last_syn] =&gt; Array\n                (\n                )\n\n            [full] =&gt; Array\n                (\n                    [0] =&gt; MIRAGE\n                    [1] =&gt; AIR\n                    [2] =&gt; CRAFT\n                    [3] =&gt; SERVICES\n                )\n\n            [full_syn] =&gt; Array\n                (\n                    [MIRAGE] =&gt; Array\n                        (\n                        )\n\n                    [AIR] =&gt; Array\n                        (\n                            [0] =&gt; AEREA\n                            [1] =&gt; AEREO\n                            [2] =&gt; AEREOS\n                            [3] =&gt; EIR\n                        )\n\n                    [CRAFT] =&gt; Array\n                        (\n                        )\n\n                    [SERVICES] =&gt; Array\n                        (\n                            [0] =&gt; SERV\n                            [1] =&gt; SERVICIO\n                            [2] =&gt; SERVICIOS\n                            [3] =&gt; SERVICOS\n                            [4] =&gt; SERVICE\n                        )\n\n                )\n\n            [icij_name] =&gt; Array\n                (\n                    [0] =&gt; MIRAGE\n                    [1] =&gt; AIR\n                    [2] =&gt; CRAFT\n                    [3] =&gt; SERVICES\n                )\n\n            [icij_nameSyn] =&gt; Array\n                (\n                    [MIRAGE] =&gt; Array\n                        (\n                        )\n\n                    [AIR] =&gt; Array\n                        (\n                            [0] =&gt; AEREA\n                            [1] =&gt; AEREO\n                            [2] =&gt; AEREOS\n                            [3] =&gt; EIR\n                        )\n\n                    [CRAFT] =&gt; Array\n                        (\n                        )\n\n                    [SERVICES] =&gt; Array\n                        (\n                            [0] =&gt; SERV\n                            [1] =&gt; SERVICIO\n                            [2] =&gt; SERVICIOS\n                            [3] =&gt; SERVICOS\n                            [4] =&gt; SERVICE\n                        )\n\n                )\n\n        )\n\n    [deflated] =&gt; MIRAGEAIRCRAFTSERVICES\n    [generated] =&gt; Array\n        (\n            [pep] =&gt; 2025-07-22 16:47:11\n            [sanction] =&gt; 2025-09-09 15:05:21\n            [watch] =&gt; 2025-08-07 17:33:59\n            [mex] =&gt; 2025-07-31 13:34:08\n            [soe] =&gt; 2025-06-18 10:36:28\n            [rights] =&gt; 2025-07-31 13:47:27\n            [col] =&gt; 2025-07-31 13:42:51\n            [icij] =&gt; 2016-07-15 00:00:00\n        )\n\n    [matches] =&gt; 2\n    [hits] =&gt; 3\n    [ref] =&gt; Array\n        (\n            [sanction] =&gt; Array\n                (\n                    [0] =&gt; 361804:10131047950\n                )\n\n            [watch] =&gt; Array\n                (\n                    [0] =&gt; 6306178:20201576120\n                    [1] =&gt; 6444316:20201633423\n                )\n\n        )\n\n    [runtime] =&gt; Array\n        (\n            [pep] =&gt; 0.007\n            [sanction] =&gt; 0.009\n            [watch] =&gt; 0.008\n            [mex] =&gt; 0.009\n            [soe] =&gt; 0.007\n            [rights] =&gt; 0.012\n            [col] =&gt; 0.009\n            [icij] =&gt; 0.006\n        )\n\n    [error] =&gt; \n    [countryExcl] =&gt; \n    [listExcl] =&gt; \n    [sqlTemplate] =&gt; SELECT DISTINCT L1.recid\nFROM {_tbl_} AS L1{filter_join}\nINNER JOIN {_tbl_} AS L2 ON L2.recid = L1.recid\nINNER JOIN {_tbl_} AS L3 ON L3.recid = L1.recid\nINNER JOIN {_tbl_} AS L4 ON L4.recid = L1.recid\nWHERE {filter_cond}L1.token = 'MIRAGE'\nAND (L2.token = 'AIR'\n  OR L2.token = 'AEREA'\n  OR L2.token = 'AEREO'\n  OR L2.token = 'AEREOS'\n  OR L2.token = 'EIR'\n)\nAND L3.token = 'CRAFT'\nAND (L4.token = 'SERVICES'\n  OR L4.token = 'SERV'\n  OR L4.token = 'SERVICIO'\n  OR L4.token = 'SERVICIOS'\n  OR L4.token = 'SERVICOS'\n  OR L4.token = 'SERVICE'\n)\nLIMIT 100\n    [deflatedSqlTemplate] =&gt; SELECT DISTINCT L1.recid\nFROM {_tbl_} AS L1{filter_join}\nWHERE {filter_cond}L1.token = 'MIRAGEAIRCRAFTSERVICES'\nAND L1.nameSrc = 'Deflated'\n LIMIT 100\n    [nameID] =&gt; 3341266\n    [icijName] =&gt; Mirage Air craft Services\n    [sqlTemplate_icij] =&gt; SELECT DISTINCT L1.recid\nFROM {_tbl_} AS L1\nINNER JOIN {_tbl_} AS L2 ON L2.recid = L1.recid\nINNER JOIN {_tbl_} AS L3 ON L3.recid = L1.recid\nINNER JOIN {_tbl_} AS L4 ON L4.recid = L1.recid\nLEFT JOIN {_tbl_} AS deflateJoin ON deflateJoin.recid = L1.recid\nWHERE L1.token = 'MIRAGE'\nAND (L2.token = 'AIR'\n  OR L2.token = 'AEREA'\n  OR L2.token = 'AEREO'\n  OR L2.token = 'AEREOS'\n  OR L2.token = 'EIR'\n)\nAND L3.token = 'CRAFT'\nAND (L4.token = 'SERVICES'\n  OR L4.token = 'SERV'\n  OR L4.token = 'SERVICIO'\n  OR L4.token = 'SERVICIOS'\n  OR L4.token = 'SERVICOS'\n  OR L4.token = 'SERVICE'\n)\nAND deflateJoin.token LIKE '%MIRAGEAIRCRAFTSERVICES%'\nLIMIT 100\n)\n","Preview":{"pep":[],"sanction":[{"recid":361804,"ID":"10131047950","First_Name":"","Last_Name":"MIRAGE AIR CRAFT SERVICES SOLE PROPRIETORSHIP LLC","Full_Name":"","Other_Names":"","AltScript":"","RecType":"E"}],"watch":[{"recid":6306178,"ID":"20201576120","First_Name":"","Last_Name":"","Full_Name":"MIRAGE AIR CRAFT SERVICES SOLE PROPREITORSHIP LLC","Other_Names":"","AltScript":"","RecType":"E"},{"recid":6444316,"ID":"20201633423","First_Name":"","Last_Name":"","Full_Name":"MIRAGE AIR CRAFT SERVICES SOLE PROPRIETORSHIP LLC","Other_Names":"","AltScript":"","RecType":"E"}],"icij":[],"mex":[],"soe":[],"rights":[],"col":[],"media":[],"ofac":[]}}}],"Redirect":null}</t>
+  </si>
+  <si>
+    <t>BroadCom Wireless Communications Corporation</t>
+  </si>
+  <si>
+    <t>{"Result":1,"ErrTitle":"","ErrMsg":"","ErrMsgWidth":null,"ErrBtnLabel":"Ok","MultiErr":null,"AppNotice":null,"FuncName":null,"Args":[{"nameSearch":{"SearchResult":{"timestamp":"2025-09-17 14:35:05","firstName":"","lastName":"","fullName":"BroadCom Wireless Communications Corporation","type":"E","method":3,"tokens":{"first":[],"first_syn":[],"last":[],"last_syn":[],"full":["BROADCOM","WIRELESS","COMMUNICATIONS"],"full_syn":{"BROADCOM":[],"WIRELESS":[],"COMMUNICATIONS":[]},"icij_name":["BROADCOM","WIRELESS","COMMUNICATIONS"],"icij_nameSyn":{"BROADCOM":[],"WIRELESS":[],"COMMUNICATIONS":[]}},"deflated":"BROADCOMWIRELESSCOMMUNICATIONSCORPORATION","generated":{"pep":"2025-07-22 16:47:11","sanction":"2025-09-09 15:05:21","watch":"2025-08-07 17:33:59","mex":"2025-07-31 13:34:08","soe":"2025-06-18 10:36:28","rights":"2025-07-31 13:47:27","col":"2025-07-31 13:42:51","icij":"2016-07-15 00:00:00"},"matches":1,"hits":1,"ref":{"watch":["3319709:20200616696"]},"runtime":{"pep":0.01400000000000000029143354396410359186120331287384033203125,"sanction":0.0290000000000000014710455076283324160613119602203369140625,"watch":0.0259999999999999988065102485279567190445959568023681640625,"mex":0.0189999999999999995281552145343084703199565410614013671875,"soe":0.0259999999999999988065102485279567190445959568023681640625,"rights":0.00899999999999999931998839741709161899052560329437255859375,"col":0.007000000000000000145716771982051795930601656436920166015625,"icij":0.01000000000000000020816681711721685132943093776702880859375},"error":"","countryExcl":"","listExcl":"","sqlTemplate":"SELECT DISTINCT L1.recid\nFROM {_tbl_} AS L1{filter_join}\nINNER JOIN {_tbl_} AS L2 ON L2.recid = L1.recid\nINNER JOIN {_tbl_} AS L3 ON L3.recid = L1.recid\nWHERE {filter_cond}L1.token = 'BROADCOM'\nAND L2.token = 'WIRELESS'\nAND L3.token = 'COMMUNICATIONS'\nLIMIT 100","deflatedSqlTemplate":"SELECT DISTINCT L1.recid\nFROM {_tbl_} AS L1{filter_join}\nWHERE {filter_cond}L1.token = 'BROADCOMWIRELESSCOMMUNICATIONSCORPORATION'\nAND L1.nameSrc = 'Deflated'\n LIMIT 100","nameID":3556807,"icijName":"BroadCom Wireless Communications Corporation","sqlTemplate_icij":"SELECT DISTINCT L1.recid\nFROM {_tbl_} AS L1\nINNER JOIN {_tbl_} AS L2 ON L2.recid = L1.recid\nINNER JOIN {_tbl_} AS L3 ON L3.recid = L1.recid\nLEFT JOIN {_tbl_} AS deflateJoin ON deflateJoin.recid = L1.recid\nWHERE L1.token = 'BROADCOM'\nAND L2.token = 'WIRELESS'\nAND L3.token = 'COMMUNICATIONS'\nAND deflateJoin.token LIKE '%BROADCOMWIRELESSCOMMUNICATIONSCORPORATION%'\nLIMIT 100"},"code":"Array\n(\n    [timestamp] =&gt; 2025-09-17 14:35:05\n    [firstName] =&gt; \n    [lastName] =&gt; \n    [fullName] =&gt; BroadCom Wireless Communications Corporation\n    [type] =&gt; E\n    [method] =&gt; 3\n    [tokens] =&gt; Array\n        (\n            [first] =&gt; Array\n                (\n                )\n\n            [first_syn] =&gt; Array\n                (\n                )\n\n            [last] =&gt; Array\n                (\n                )\n\n            [last_syn] =&gt; Array\n                (\n                )\n\n            [full] =&gt; Array\n                (\n                    [0] =&gt; BROADCOM\n                    [1] =&gt; WIRELESS\n                    [2] =&gt; COMMUNICATIONS\n                )\n\n            [full_syn] =&gt; Array\n                (\n                    [BROADCOM] =&gt; Array\n                        (\n                        )\n\n                    [WIRELESS] =&gt; Array\n                        (\n                        )\n\n                    [COMMUNICATIONS] =&gt; Array\n                        (\n                        )\n\n                )\n\n            [icij_name] =&gt; Array\n                (\n                    [0] =&gt; BROADCOM\n                    [1] =&gt; WIRELESS\n                    [2] =&gt; COMMUNICATIONS\n                )\n\n            [icij_nameSyn] =&gt; Array\n                (\n                    [BROADCOM] =&gt; Array\n                        (\n                        )\n\n                    [WIRELESS] =&gt; Array\n                        (\n                        )\n\n                    [COMMUNICATIONS] =&gt; Array\n                        (\n                        )\n\n                )\n\n        )\n\n    [deflated] =&gt; BROADCOMWIRELESSCOMMUNICATIONSCORPORATION\n    [generated] =&gt; Array\n        (\n            [pep] =&gt; 2025-07-22 16:47:11\n            [sanction] =&gt; 2025-09-09 15:05:21\n            [watch] =&gt; 2025-08-07 17:33:59\n            [mex] =&gt; 2025-07-31 13:34:08\n            [soe] =&gt; 2025-06-18 10:36:28\n            [rights] =&gt; 2025-07-31 13:47:27\n            [col] =&gt; 2025-07-31 13:42:51\n            [icij] =&gt; 2016-07-15 00:00:00\n        )\n\n    [matches] =&gt; 1\n    [hits] =&gt; 1\n    [ref] =&gt; Array\n        (\n            [watch] =&gt; Array\n                (\n                    [0] =&gt; 3319709:20200616696\n                )\n\n        )\n\n    [runtime] =&gt; Array\n        (\n            [pep] =&gt; 0.014\n            [sanction] =&gt; 0.029\n            [watch] =&gt; 0.026\n            [mex] =&gt; 0.019\n            [soe] =&gt; 0.026\n            [rights] =&gt; 0.009\n            [col] =&gt; 0.007\n            [icij] =&gt; 0.01\n        )\n\n    [error] =&gt; \n    [countryExcl] =&gt; \n    [listExcl] =&gt; \n    [sqlTemplate] =&gt; SELECT DISTINCT L1.recid\nFROM {_tbl_} AS L1{filter_join}\nINNER JOIN {_tbl_} AS L2 ON L2.recid = L1.recid\nINNER JOIN {_tbl_} AS L3 ON L3.recid = L1.recid\nWHERE {filter_cond}L1.token = 'BROADCOM'\nAND L2.token = 'WIRELESS'\nAND L3.token = 'COMMUNICATIONS'\nLIMIT 100\n    [deflatedSqlTemplate] =&gt; SELECT DISTINCT L1.recid\nFROM {_tbl_} AS L1{filter_join}\nWHERE {filter_cond}L1.token = 'BROADCOMWIRELESSCOMMUNICATIONSCORPORATION'\nAND L1.nameSrc = 'Deflated'\n LIMIT 100\n    [nameID] =&gt; 3556807\n    [icijName] =&gt; BroadCom Wireless Communications Corporation\n    [sqlTemplate_icij] =&gt; SELECT DISTINCT L1.recid\nFROM {_tbl_} AS L1\nINNER JOIN {_tbl_} AS L2 ON L2.recid = L1.recid\nINNER JOIN {_tbl_} AS L3 ON L3.recid = L1.recid\nLEFT JOIN {_tbl_} AS deflateJoin ON deflateJoin.recid = L1.recid\nWHERE L1.token = 'BROADCOM'\nAND L2.token = 'WIRELESS'\nAND L3.token = 'COMMUNICATIONS'\nAND deflateJoin.token LIKE '%BROADCOMWIRELESSCOMMUNICATIONSCORPORATION%'\nLIMIT 100\n)\n","Preview":{"pep":[],"sanction":[],"watch":[{"recid":3319709,"ID":"20200616696","First_Name":"","Last_Name":"","Full_Name":"BroadCom Wireless Communications Corporation","Other_Names":"","AltScript":"","RecType":"E"}],"icij":[],"mex":[],"soe":[],"rights":[],"col":[],"media":[],"ofac":[]}}}],"Redirect":null}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +182,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -207,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -221,6 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,16 +544,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="84" customWidth="1"/>
-    <col min="3" max="3" width="57.33203125" customWidth="1"/>
+    <col min="3" max="3" width="93.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -580,172 +601,194 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
+      <c r="A5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
+      <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>